<commit_message>
fixing number of exluded
</commit_message>
<xml_diff>
--- a/HEAT_Tables_0517_am.xlsx
+++ b/HEAT_Tables_0517_am.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wrhiza-my.sharepoint.com/personal/cparker_wrhi_ac_za/Documents/Desktop/Heat_Project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{174E8CE6-EB2B-48E5-B8A1-EF65EB64FB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A13B4F5-9AD3-4D45-A8D7-FCEF69F90D7B}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{174E8CE6-EB2B-48E5-B8A1-EF65EB64FB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CCE5EF3-D91F-455B-B916-9C1893B43A05}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{91FD6BB3-C241-4A4C-A7CD-77275B6BC45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{91FD6BB3-C241-4A4C-A7CD-77275B6BC45F}"/>
   </bookViews>
   <sheets>
     <sheet name="RP1" sheetId="3" r:id="rId1"/>
@@ -806,9 +806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2136BA5-E5C5-47AA-8FB2-ABBFBE69B251}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R2" sqref="R2:R10"/>
+      <selection pane="topRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,7 +926,7 @@
         <v>58</v>
       </c>
       <c r="R2" s="21">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -1374,7 +1374,7 @@
         <v>36</v>
       </c>
       <c r="R10" s="21">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1823,7 +1823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EEDAFB-5DD9-4712-8169-3CA90A65D01B}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="L2" sqref="L2"/>
     </sheetView>
@@ -2735,11 +2735,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="84e45b98-9724-46df-936f-ec42a4cf951b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2996,20 +2997,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="84e45b98-9724-46df-936f-ec42a4cf951b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29346A3B-E74B-4386-AD79-218823B89808}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{402FBE93-6AD6-436A-9711-D8E18344BF8D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="84e45b98-9724-46df-936f-ec42a4cf951b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3034,9 +3032,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{402FBE93-6AD6-436A-9711-D8E18344BF8D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29346A3B-E74B-4386-AD79-218823B89808}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="84e45b98-9724-46df-936f-ec42a4cf951b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>